<commit_message>
Update Scripts Cancellazione, sales
</commit_message>
<xml_diff>
--- a/docs/tp/Navigation.xlsx
+++ b/docs/tp/Navigation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A826360C-8612-4135-AA67-367DA85D4F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C0373B-85A0-49D1-9B4E-20AF25100BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="810" windowWidth="19440" windowHeight="15000" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
+    <workbookView xWindow="-19320" yWindow="660" windowWidth="19440" windowHeight="15000" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="319">
   <si>
     <t>Design</t>
   </si>
@@ -912,6 +912,84 @@
   </si>
   <si>
     <t>click sul pannello "Notifiche in evidenza" e verifica la presenza delle notifiche</t>
+  </si>
+  <si>
+    <t>Verifica Top Menu incident - Verifica atterraggio SRM Online</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_HomePage_Verifica Top Menu incident - Verifica atterraggio SRM Online</t>
+  </si>
+  <si>
+    <t>Click icona incident dai top Menu, click sul link SRM Online e verifica atterraggio</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_HomePage_Verifica Top Menu incident - Verifica atterraggio SisCo</t>
+  </si>
+  <si>
+    <t>Verifica Top Menu incident - Verifica atterraggio SisCo</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_HomePage_Verifica Top Menu incident - Verifica atterraggio Elenco telefonico</t>
+  </si>
+  <si>
+    <t>Verifica Top Menu incident - Verifica atterraggio Elenco telefonico</t>
+  </si>
+  <si>
+    <t>Click icona incident dai top Menu, click sul link Elenco telefonico e verifica atterraggio</t>
+  </si>
+  <si>
+    <t>Verifica atterraggio da Utility - Cruscotto resilience</t>
+  </si>
+  <si>
+    <t>Verifica atterraggio da Utility - Quattroruote - Calcolo valore veicolo</t>
+  </si>
+  <si>
+    <t>Verifica atterraggio da Utility - Interrogazioni centralizzate</t>
+  </si>
+  <si>
+    <t>Verifica atterraggio da Utility - Banche Dati ANIA</t>
+  </si>
+  <si>
+    <t>Verifica atterraggio da Utility - Gestione Magazzino OBU</t>
+  </si>
+  <si>
+    <t>Verifica atterraggio da Utility - Cruscotto Installazione Dispositivo Satellitare</t>
+  </si>
+  <si>
+    <t>Verifica atterraggio da Utility - Monitor Scoring AZ Bonus Drive</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_HomePage_Verifica atterraggio da Utility - Quattroruote - Calcolo valore veicolo</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_HomePage_Verifica atterraggio da Utility - Interrogazioni centralizzate</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_HomePage_Verifica atterraggio da Utility - Banche Dati ANIA</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_HomePage_Verifica atterraggio da Utility - Gestione Magazzino OBU</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_HomePage_Verifica atterraggio da Utility - Cruscotto Installazione Dispositivo Satellitare</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_HomePage_Verifica atterraggio da Utility - Monitor Scoring AZ Bonus Drive</t>
+  </si>
+  <si>
+    <t>Click icona SwitchBurger dai top Menu, click sul link Utilità e verifica atterraggio della pagina</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_HomePage_Verifica atterraggio da Utility - Cruscotto resilience</t>
+  </si>
+  <si>
+    <t>Verifica presenza links da Utility</t>
+  </si>
+  <si>
+    <t>Click icona SwitchBurger dai top Menu, click sul link Utilità e verifica la presenza dei link</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_HomePage_Verifica presenza links da Utility</t>
   </si>
 </sst>
 </file>
@@ -1327,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AEFEBA-728D-4FDD-9B3D-F6BE0E3793BC}">
-  <dimension ref="A1:J113"/>
+  <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N101" sqref="N101"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4069,13 +4147,13 @@
     </row>
     <row r="86" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>191</v>
+        <v>294</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>190</v>
+        <v>293</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>203</v>
+        <v>295</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>15</v>
@@ -4101,13 +4179,13 @@
     </row>
     <row r="87" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>192</v>
+        <v>296</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>184</v>
+        <v>297</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>204</v>
+        <v>295</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>15</v>
@@ -4133,13 +4211,13 @@
     </row>
     <row r="88" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>194</v>
+        <v>298</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>195</v>
+        <v>299</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>205</v>
+        <v>300</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>15</v>
@@ -4165,13 +4243,13 @@
     </row>
     <row r="89" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>197</v>
+        <v>318</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>261</v>
+        <v>316</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>262</v>
+        <v>317</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>15</v>
@@ -4197,13 +4275,13 @@
     </row>
     <row r="90" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>196</v>
+        <v>315</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>193</v>
+        <v>301</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>206</v>
+        <v>314</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>15</v>
@@ -4229,13 +4307,13 @@
     </row>
     <row r="91" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>199</v>
+        <v>308</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>198</v>
+        <v>302</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>207</v>
+        <v>314</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>15</v>
@@ -4261,13 +4339,13 @@
     </row>
     <row r="92" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>201</v>
+        <v>309</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>200</v>
+        <v>303</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>208</v>
+        <v>314</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>15</v>
@@ -4293,13 +4371,13 @@
     </row>
     <row r="93" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>229</v>
+        <v>310</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>228</v>
+        <v>304</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>202</v>
+        <v>314</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>15</v>
@@ -4325,13 +4403,13 @@
     </row>
     <row r="94" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>209</v>
+        <v>311</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>210</v>
+        <v>305</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>211</v>
+        <v>314</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>15</v>
@@ -4357,13 +4435,13 @@
     </row>
     <row r="95" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>212</v>
+        <v>312</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>213</v>
+        <v>306</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>220</v>
+        <v>314</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>15</v>
@@ -4389,13 +4467,13 @@
     </row>
     <row r="96" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>214</v>
+        <v>313</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>215</v>
+        <v>307</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>221</v>
+        <v>314</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>15</v>
@@ -4421,13 +4499,13 @@
     </row>
     <row r="97" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>216</v>
+        <v>191</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>15</v>
@@ -4453,13 +4531,13 @@
     </row>
     <row r="98" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>219</v>
+        <v>184</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>15</v>
@@ -4485,13 +4563,13 @@
     </row>
     <row r="99" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>288</v>
+        <v>194</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>287</v>
+        <v>195</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>15</v>
@@ -4517,13 +4595,13 @@
     </row>
     <row r="100" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>225</v>
+        <v>261</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>227</v>
+        <v>262</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>15</v>
@@ -4549,13 +4627,13 @@
     </row>
     <row r="101" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>291</v>
+        <v>196</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>290</v>
+        <v>193</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>292</v>
+        <v>206</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>15</v>
@@ -4581,385 +4659,737 @@
     </row>
     <row r="102" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J102" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H103" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J103" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J104" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H105" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J105" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J106" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H107" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I107" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J107" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H108" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J108" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H109" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I109" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J109" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J110" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H111" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J111" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J112" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B113" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="C113" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="D102" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F102" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G102" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H102" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I102" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J102" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
+      <c r="D113" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H113" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J113" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B114" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C114" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="D103" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G103" s="3" t="s">
+      <c r="D114" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G114" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H103" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I103" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J103" s="3" t="s">
+      <c r="H114" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J114" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
+    <row r="115" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B115" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C115" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D104" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G104" s="3" t="s">
+      <c r="D115" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G115" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H104" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I104" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J104" s="3" t="s">
+      <c r="H115" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J115" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="s">
+    <row r="116" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B116" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="C116" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G105" s="3" t="s">
+      <c r="D116" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G116" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H105" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I105" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J105" s="3" t="s">
+      <c r="H116" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J116" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
+    <row r="117" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B117" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C117" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D106" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F106" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G106" s="3" t="s">
+      <c r="D117" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G117" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H106" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I106" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J106" s="3" t="s">
+      <c r="H117" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J117" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
+    <row r="118" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B118" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C118" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D107" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F107" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G107" s="3" t="s">
+      <c r="D118" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G118" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H107" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I107" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J107" s="3" t="s">
+      <c r="H118" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J118" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
+    <row r="119" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B119" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C119" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D108" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F108" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G108" s="3" t="s">
+      <c r="D119" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G119" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H108" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I108" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J108" s="3" t="s">
+      <c r="H119" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J119" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
+    <row r="120" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B120" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="C120" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F109" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G109" s="3" t="s">
+      <c r="D120" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G120" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H109" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I109" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J109" s="3" t="s">
+      <c r="H120" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J120" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
+    <row r="121" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B121" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="C121" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="D110" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F110" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G110" s="3" t="s">
+      <c r="D121" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G121" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H110" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I110" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J110" s="3" t="s">
+      <c r="H121" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J121" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
+    <row r="122" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B122" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="C122" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="D111" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G111" s="3" t="s">
+      <c r="D122" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G122" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H111" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I111" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J111" s="3" t="s">
+      <c r="H122" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J122" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
+    <row r="123" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B123" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="C123" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D112" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E112" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G112" s="3" t="s">
+      <c r="D123" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G123" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H112" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I112" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J112" s="3" t="s">
+      <c r="H123" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J123" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
+    <row r="124" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B124" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="C124" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="D113" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G113" s="3" t="s">
+      <c r="D124" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G124" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H113" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I113" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J113" s="3" t="s">
+      <c r="H124" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J124" s="3" t="s">
         <v>260</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Verifica Sotto pagine "Le mie info"
</commit_message>
<xml_diff>
--- a/docs/tp/Navigation.xlsx
+++ b/docs/tp/Navigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE351210-A226-4AED-BF00-A00FD27E0FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009E3689-327B-4DA3-B5A7-A70AD07E7BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="810" windowWidth="19440" windowHeight="15000" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="345">
   <si>
     <t>Design</t>
   </si>
@@ -557,12 +557,6 @@
     <t>Matrix Web : Navigation_MieInfo_Verifica aggancio Antiriciclaggio</t>
   </si>
   <si>
-    <t>Matrix Web : Navigation_MieInfo_Verifica aggancio Risorse per l\'Agenzia</t>
-  </si>
-  <si>
-    <t>Verifica aggancio Risorse per l\'Agenzia</t>
-  </si>
-  <si>
     <t>Verifica aggancio Operatività</t>
   </si>
   <si>
@@ -1005,6 +999,75 @@
   </si>
   <si>
     <t>Matrix Web : Navigation_MieInfo_Verifica aggancio New Company Handbook</t>
+  </si>
+  <si>
+    <t>Verifica aggancio su tutte le sotto pagine di Prodotti</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_MieInfo_Verifica aggancio su tutte le sotto pagine di Prodotti</t>
+  </si>
+  <si>
+    <t>Si accede a Le mie Info, verifica l'atterraggio della pagina Prodotti e l'atterraggio di tutte le sue sotto pagine</t>
+  </si>
+  <si>
+    <t>Verifica aggancio su tutte le sotto pagine di Iniziative</t>
+  </si>
+  <si>
+    <t>Si accede a Le mie Info, verifica l'atterraggio della pagina Iniziative e l'atterraggio di tutte le sue sotto pagine</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_MieInfo_Verifica aggancio su tutte le sotto pagine di Iniziative</t>
+  </si>
+  <si>
+    <t>Verifica aggancio su tutte le sotto pagine di Sales Academy</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_MieInfo_Verifica aggancio su tutte le sotto pagine di Sales Academy</t>
+  </si>
+  <si>
+    <t>Si accede a Le mie Info, verifica l'atterraggio della pagina Sales Academy e l'atterraggio di tutte le sue sotto pagine</t>
+  </si>
+  <si>
+    <t>Verifica aggancio su tutte le sotto pagine di Antiriciclaggio</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_MieInfo_Verifica aggancio su tutte le sotto pagine di Antiriciclaggio</t>
+  </si>
+  <si>
+    <t>Verifica aggancio su tutte le sotto pagine di Risorse per l'Agenzia</t>
+  </si>
+  <si>
+    <t>Si accede a Le mie Info, verifica l'atterraggio della pagina Risorse per l'Agenzia e l'atterraggio di tutte le sue sotto pagine</t>
+  </si>
+  <si>
+    <t>Si accede a Le mie Info, verifica l'atterraggio della pagina Antiriciclaggio e l'atterraggio di tutte le sue sotto pagine</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_MieInfo_Verifica aggancio su tutte le sotto pagine di Risorse per l'Agenzia</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_MieInfo_Verifica aggancio Risorse per l'Agente</t>
+  </si>
+  <si>
+    <t>Verifica aggancio Risorse per l'Agente</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_MieInfo_Verifica aggancio su tutte le sotto pagine di Risorse per l'Agente</t>
+  </si>
+  <si>
+    <t>Verifica aggancio su tutte le sotto pagine di Risorse per l'Agente</t>
+  </si>
+  <si>
+    <t>Si accede a Le mie Info, verifica l'atterraggio della pagina Risorse per l'Agente e l'atterraggio di tutte le sue sotto pagine</t>
+  </si>
+  <si>
+    <t>Verifica aggancio su tutte le sotto pagine di Il Mondo Allianz</t>
+  </si>
+  <si>
+    <t>Si accede a Le mie Info, verifica l'atterraggio della pagina Il Mondo Allianz e l'atterraggio di tutte le sue sotto pagine</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_MieInfo_Verifica aggancio su tutte le sotto pagine di Il Mondo Allianz</t>
   </si>
 </sst>
 </file>
@@ -1420,10 +1483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AEFEBA-728D-4FDD-9B3D-F6BE0E3793BC}">
-  <dimension ref="A1:J126"/>
+  <dimension ref="A1:J133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1925,7 +1988,7 @@
         <v>91</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>31</v>
@@ -1957,7 +2020,7 @@
         <v>92</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>33</v>
@@ -1989,7 +2052,7 @@
         <v>93</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>34</v>
@@ -2530,10 +2593,10 @@
     </row>
     <row r="35" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>31</v>
@@ -3112,7 +3175,7 @@
         <v>68</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>15</v>
@@ -3144,7 +3207,7 @@
         <v>69</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>15</v>
@@ -3176,7 +3239,7 @@
         <v>70</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>15</v>
@@ -3240,7 +3303,7 @@
         <v>72</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>15</v>
@@ -3272,7 +3335,7 @@
         <v>73</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>15</v>
@@ -3298,13 +3361,13 @@
     </row>
     <row r="59" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>268</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>270</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>15</v>
@@ -3336,7 +3399,7 @@
         <v>74</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>15</v>
@@ -3368,7 +3431,7 @@
         <v>75</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>15</v>
@@ -3394,13 +3457,13 @@
     </row>
     <row r="62" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>279</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>15</v>
@@ -3432,7 +3495,7 @@
         <v>76</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>15</v>
@@ -3490,13 +3553,13 @@
     </row>
     <row r="65" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>15</v>
@@ -3618,10 +3681,10 @@
     </row>
     <row r="69" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>159</v>
@@ -3680,47 +3743,33 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>155</v>
+        <v>323</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>156</v>
+        <v>322</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I71" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J71" s="3" t="s">
-        <v>139</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
     </row>
     <row r="72" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>15</v>
@@ -3744,47 +3793,33 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>161</v>
+        <v>327</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>160</v>
+        <v>325</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H73" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I73" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J73" s="3" t="s">
-        <v>139</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
     </row>
     <row r="74" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>15</v>
@@ -3810,13 +3845,13 @@
     </row>
     <row r="75" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>15</v>
@@ -3840,47 +3875,33 @@
         <v>139</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>168</v>
+        <v>329</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>167</v>
+        <v>328</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G76" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H76" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I76" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J76" s="3" t="s">
-        <v>139</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
     </row>
     <row r="77" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>15</v>
@@ -3906,13 +3927,13 @@
     </row>
     <row r="78" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>323</v>
+        <v>164</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>322</v>
+        <v>165</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>15</v>
@@ -3938,13 +3959,13 @@
     </row>
     <row r="79" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>15</v>
@@ -3970,13 +3991,13 @@
     </row>
     <row r="80" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>24</v>
+        <v>170</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>15</v>
@@ -4002,10 +4023,10 @@
     </row>
     <row r="81" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>174</v>
+        <v>321</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>175</v>
+        <v>320</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>159</v>
@@ -4034,13 +4055,13 @@
     </row>
     <row r="82" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>15</v>
@@ -4066,10 +4087,10 @@
     </row>
     <row r="83" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>179</v>
+        <v>24</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>159</v>
@@ -4096,47 +4117,33 @@
         <v>139</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>180</v>
+        <v>332</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>181</v>
+        <v>331</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H84" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I84" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J84" s="3" t="s">
-        <v>139</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
     </row>
     <row r="85" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>15</v>
@@ -4160,47 +4167,33 @@
         <v>139</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>185</v>
+        <v>336</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>184</v>
+        <v>333</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J86" s="3" t="s">
-        <v>139</v>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
     </row>
     <row r="87" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>263</v>
+        <v>166</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>15</v>
@@ -4226,13 +4219,13 @@
     </row>
     <row r="88" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>292</v>
+        <v>337</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>291</v>
+        <v>338</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>293</v>
+        <v>159</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>15</v>
@@ -4256,47 +4249,33 @@
         <v>139</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>294</v>
+        <v>339</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>295</v>
+        <v>340</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F89" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I89" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J89" s="3" t="s">
-        <v>139</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
     </row>
     <row r="90" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>296</v>
+        <v>178</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>297</v>
+        <v>179</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>298</v>
+        <v>159</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>15</v>
@@ -4320,47 +4299,33 @@
         <v>139</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>316</v>
+        <v>344</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>314</v>
+        <v>342</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G91" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H91" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I91" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J91" s="3" t="s">
-        <v>139</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
     </row>
     <row r="92" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>313</v>
+        <v>181</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>299</v>
+        <v>180</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>312</v>
+        <v>184</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>15</v>
@@ -4386,13 +4351,13 @@
     </row>
     <row r="93" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>306</v>
+        <v>183</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>300</v>
+        <v>182</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>312</v>
+        <v>185</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>15</v>
@@ -4418,13 +4383,13 @@
     </row>
     <row r="94" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>307</v>
+        <v>187</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>301</v>
+        <v>186</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>312</v>
+        <v>261</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>15</v>
@@ -4450,13 +4415,13 @@
     </row>
     <row r="95" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>312</v>
+        <v>291</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>15</v>
@@ -4482,13 +4447,13 @@
     </row>
     <row r="96" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>312</v>
+        <v>291</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>15</v>
@@ -4514,13 +4479,13 @@
     </row>
     <row r="97" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>15</v>
@@ -4546,13 +4511,13 @@
     </row>
     <row r="98" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>15</v>
@@ -4578,13 +4543,13 @@
     </row>
     <row r="99" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>191</v>
+        <v>311</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>190</v>
+        <v>297</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>203</v>
+        <v>310</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>15</v>
@@ -4610,13 +4575,13 @@
     </row>
     <row r="100" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>192</v>
+        <v>304</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>184</v>
+        <v>298</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>204</v>
+        <v>310</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>15</v>
@@ -4642,13 +4607,13 @@
     </row>
     <row r="101" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>194</v>
+        <v>305</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>195</v>
+        <v>299</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>205</v>
+        <v>310</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>15</v>
@@ -4674,13 +4639,13 @@
     </row>
     <row r="102" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>197</v>
+        <v>306</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>259</v>
+        <v>300</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>260</v>
+        <v>310</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>15</v>
@@ -4706,13 +4671,13 @@
     </row>
     <row r="103" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>196</v>
+        <v>307</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>193</v>
+        <v>301</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>206</v>
+        <v>310</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>15</v>
@@ -4738,13 +4703,13 @@
     </row>
     <row r="104" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>199</v>
+        <v>308</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>198</v>
+        <v>302</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>207</v>
+        <v>310</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>15</v>
@@ -4770,13 +4735,13 @@
     </row>
     <row r="105" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>201</v>
+        <v>309</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>200</v>
+        <v>303</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>208</v>
+        <v>310</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>15</v>
@@ -4802,13 +4767,13 @@
     </row>
     <row r="106" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>229</v>
+        <v>189</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>228</v>
+        <v>188</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>15</v>
@@ -4834,13 +4799,13 @@
     </row>
     <row r="107" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>15</v>
@@ -4866,13 +4831,13 @@
     </row>
     <row r="108" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>15</v>
@@ -4898,13 +4863,13 @@
     </row>
     <row r="109" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>215</v>
+        <v>257</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>15</v>
@@ -4930,13 +4895,13 @@
     </row>
     <row r="110" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>217</v>
+        <v>191</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>15</v>
@@ -4962,13 +4927,13 @@
     </row>
     <row r="111" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>15</v>
@@ -4994,13 +4959,13 @@
     </row>
     <row r="112" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>286</v>
+        <v>199</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>285</v>
+        <v>198</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>15</v>
@@ -5026,13 +4991,13 @@
     </row>
     <row r="113" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>227</v>
+        <v>200</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>15</v>
@@ -5058,13 +5023,13 @@
     </row>
     <row r="114" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>289</v>
+        <v>207</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>288</v>
+        <v>208</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>290</v>
+        <v>209</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>15</v>
@@ -5090,205 +5055,205 @@
     </row>
     <row r="115" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H115" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J115" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H117" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J117" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J118" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B119" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C119" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H119" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J119" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J120" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F115" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G115" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H115" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I115" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J115" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F116" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G116" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H116" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I116" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J116" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E117" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F117" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G117" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H117" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I117" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J117" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E118" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F118" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G118" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H118" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I118" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J118" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F119" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G119" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H119" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I119" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J119" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E120" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F120" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G120" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H120" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I120" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J120" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
-        <v>242</v>
-      </c>
       <c r="B121" s="3" t="s">
-        <v>241</v>
+        <v>286</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>245</v>
+        <v>288</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>15</v>
@@ -5300,7 +5265,7 @@
         <v>1</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>140</v>
+        <v>13</v>
       </c>
       <c r="H121" s="3" t="s">
         <v>12</v>
@@ -5309,18 +5274,18 @@
         <v>2</v>
       </c>
       <c r="J121" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>243</v>
+        <v>282</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>244</v>
+        <v>281</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>248</v>
+        <v>285</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>15</v>
@@ -5332,7 +5297,7 @@
         <v>1</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>140</v>
+        <v>13</v>
       </c>
       <c r="H122" s="3" t="s">
         <v>12</v>
@@ -5341,18 +5306,18 @@
         <v>2</v>
       </c>
       <c r="J122" s="3" t="s">
-        <v>258</v>
+        <v>139</v>
       </c>
     </row>
     <row r="123" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>15</v>
@@ -5373,18 +5338,18 @@
         <v>2</v>
       </c>
       <c r="J123" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="124" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>15</v>
@@ -5405,18 +5370,18 @@
         <v>2</v>
       </c>
       <c r="J124" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="125" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>15</v>
@@ -5437,18 +5402,18 @@
         <v>2</v>
       </c>
       <c r="J125" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="126" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>317</v>
+        <v>237</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>318</v>
+        <v>236</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>15</v>
@@ -5469,7 +5434,231 @@
         <v>2</v>
       </c>
       <c r="J126" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F127" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H127" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J127" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J128" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H129" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I129" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J129" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J130" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G131" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H131" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I131" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J131" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J132" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G133" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H133" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J133" s="3" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Navigation Monitoraggio Carico
</commit_message>
<xml_diff>
--- a/docs/tp/Navigation.xlsx
+++ b/docs/tp/Navigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78D6A62-74B3-4EA3-80A9-12FA57D81537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7686E10E-F1E5-42FC-81B0-EE524E93D60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="660" windowWidth="19440" windowHeight="15000" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1990" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="514">
   <si>
     <t>Design</t>
   </si>
@@ -1592,6 +1592,15 @@
   </si>
   <si>
     <t xml:space="preserve">Verifica aggancio della pagina Unico verificando che gli aggiornamenti unico siano presenti </t>
+  </si>
+  <si>
+    <t>Verifica su Indicatori Operativi aggancio  Monitoraggio carico</t>
+  </si>
+  <si>
+    <t>Matrix Web : Navigation_Numbers_Verifica su Indicatori Operativi aggancio  Monitoraggio carico</t>
+  </si>
+  <si>
+    <t>Si accede a Numbers, click sul tab Indicatori Operativi, verifica l'atterraggio alla pagina del primo indice di monitoraggio carico</t>
   </si>
 </sst>
 </file>
@@ -2106,10 +2115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AEFEBA-728D-4FDD-9B3D-F6BE0E3793BC}">
-  <dimension ref="A1:J199"/>
+  <dimension ref="A1:J200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:XFD65"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4334,7 +4343,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>128</v>
       </c>
@@ -4366,7 +4375,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>259</v>
       </c>
@@ -4398,7 +4407,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>129</v>
       </c>
@@ -4430,7 +4439,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>130</v>
       </c>
@@ -4462,7 +4471,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>283</v>
       </c>
@@ -4494,7 +4503,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>138</v>
       </c>
@@ -4526,7 +4535,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>142</v>
       </c>
@@ -4558,7 +4567,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>145</v>
       </c>
@@ -4590,7 +4599,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>256</v>
       </c>
@@ -4622,7 +4631,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>148</v>
       </c>
@@ -4654,7 +4663,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>287</v>
       </c>
@@ -4686,7 +4695,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>149</v>
       </c>
@@ -4718,7 +4727,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>291</v>
       </c>
@@ -4750,7 +4759,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>151</v>
       </c>
@@ -4782,7 +4791,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>155</v>
       </c>
@@ -4814,7 +4823,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>293</v>
       </c>
@@ -4878,7 +4887,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>158</v>
       </c>
@@ -4910,7 +4919,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>162</v>
       </c>
@@ -4942,7 +4951,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>163</v>
       </c>
@@ -4974,7 +4983,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>285</v>
       </c>
@@ -5006,7 +5015,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>166</v>
       </c>
@@ -5038,7 +5047,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>167</v>
       </c>
@@ -5070,7 +5079,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>296</v>
       </c>
@@ -5102,7 +5111,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>170</v>
       </c>
@@ -5134,7 +5143,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>300</v>
       </c>
@@ -5198,7 +5207,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>301</v>
       </c>
@@ -5230,7 +5239,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>303</v>
       </c>
@@ -5262,7 +5271,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>172</v>
       </c>
@@ -5294,7 +5303,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>308</v>
       </c>
@@ -5326,7 +5335,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>175</v>
       </c>
@@ -5358,7 +5367,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>177</v>
       </c>
@@ -5390,7 +5399,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>181</v>
       </c>
@@ -5422,7 +5431,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>271</v>
       </c>
@@ -5454,7 +5463,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>273</v>
       </c>
@@ -5486,7 +5495,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>275</v>
       </c>
@@ -5518,7 +5527,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>365</v>
       </c>
@@ -5550,7 +5559,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>366</v>
       </c>
@@ -5838,7 +5847,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>183</v>
       </c>
@@ -5870,7 +5879,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>184</v>
       </c>
@@ -5902,7 +5911,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>186</v>
       </c>
@@ -5934,7 +5943,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>189</v>
       </c>
@@ -5966,7 +5975,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>188</v>
       </c>
@@ -5998,7 +6007,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>191</v>
       </c>
@@ -6030,7 +6039,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>193</v>
       </c>
@@ -6062,7 +6071,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>221</v>
       </c>
@@ -6094,7 +6103,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>201</v>
       </c>
@@ -6126,7 +6135,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>204</v>
       </c>
@@ -6158,7 +6167,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>206</v>
       </c>
@@ -6190,7 +6199,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>208</v>
       </c>
@@ -6222,7 +6231,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>210</v>
       </c>
@@ -6254,7 +6263,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>400</v>
       </c>
@@ -6286,7 +6295,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>266</v>
       </c>
@@ -6318,7 +6327,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>216</v>
       </c>
@@ -6350,7 +6359,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>268</v>
       </c>
@@ -6382,7 +6391,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>222</v>
       </c>
@@ -6414,7 +6423,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>361</v>
       </c>
@@ -6446,7 +6455,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>226</v>
       </c>
@@ -6478,7 +6487,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>229</v>
       </c>
@@ -6510,7 +6519,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>232</v>
       </c>
@@ -6542,7 +6551,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>324</v>
       </c>
@@ -6574,7 +6583,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>326</v>
       </c>
@@ -6606,7 +6615,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>327</v>
       </c>
@@ -6638,7 +6647,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>330</v>
       </c>
@@ -6670,7 +6679,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>333</v>
       </c>
@@ -6702,7 +6711,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>334</v>
       </c>
@@ -6734,7 +6743,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>336</v>
       </c>
@@ -6766,7 +6775,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>342</v>
       </c>
@@ -6798,7 +6807,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>343</v>
       </c>
@@ -6830,7 +6839,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>344</v>
       </c>
@@ -6862,7 +6871,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>346</v>
       </c>
@@ -6894,7 +6903,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>347</v>
       </c>
@@ -6926,7 +6935,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
         <v>348</v>
       </c>
@@ -6958,7 +6967,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>349</v>
       </c>
@@ -6990,7 +6999,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
         <v>351</v>
       </c>
@@ -7022,7 +7031,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>356</v>
       </c>
@@ -7054,7 +7063,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="155" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>358</v>
       </c>
@@ -7086,7 +7095,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>238</v>
       </c>
@@ -7118,15 +7127,15 @@
         <v>242</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>239</v>
+        <v>512</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>410</v>
+        <v>511</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>241</v>
+        <v>513</v>
       </c>
       <c r="D157" s="4" t="s">
         <v>15</v>
@@ -7150,15 +7159,15 @@
         <v>242</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
-        <v>408</v>
+        <v>239</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>409</v>
+        <v>241</v>
       </c>
       <c r="D158" s="4" t="s">
         <v>15</v>
@@ -7184,13 +7193,13 @@
     </row>
     <row r="159" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>280</v>
+        <v>409</v>
       </c>
       <c r="D159" s="4" t="s">
         <v>15</v>
@@ -7214,47 +7223,47 @@
         <v>242</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A160" s="9" t="s">
+    <row r="160" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A160" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="C160" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D160" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E160" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F160" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G160" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H160" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I160" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J160" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A161" s="9" t="s">
         <v>417</v>
-      </c>
-      <c r="B160" s="10" t="s">
-        <v>415</v>
-      </c>
-      <c r="C160" s="12" t="s">
-        <v>414</v>
-      </c>
-      <c r="D160" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E160" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F160" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G160" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="H160" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I160" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="J160" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="161" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A161" s="9" t="s">
-        <v>418</v>
       </c>
       <c r="B161" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="C161" s="10" t="s">
-        <v>416</v>
+      <c r="C161" s="12" t="s">
+        <v>414</v>
       </c>
       <c r="D161" s="9" t="s">
         <v>15</v>
@@ -7278,15 +7287,15 @@
         <v>131</v>
       </c>
     </row>
-    <row r="162" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A162" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B162" s="10" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="D162" s="9" t="s">
         <v>15</v>
@@ -7310,15 +7319,15 @@
         <v>131</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A163" s="9" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B163" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="C163" s="11" t="s">
-        <v>424</v>
+        <v>420</v>
+      </c>
+      <c r="C163" s="10" t="s">
+        <v>423</v>
       </c>
       <c r="D163" s="9" t="s">
         <v>15</v>
@@ -7344,13 +7353,13 @@
     </row>
     <row r="164" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A164" s="9" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B164" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="C164" s="10" t="s">
-        <v>427</v>
+        <v>422</v>
+      </c>
+      <c r="C164" s="11" t="s">
+        <v>424</v>
       </c>
       <c r="D164" s="9" t="s">
         <v>15</v>
@@ -7376,13 +7385,13 @@
     </row>
     <row r="165" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A165" s="9" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B165" s="10" t="s">
-        <v>429</v>
-      </c>
-      <c r="C165" s="11" t="s">
-        <v>430</v>
+        <v>426</v>
+      </c>
+      <c r="C165" s="10" t="s">
+        <v>427</v>
       </c>
       <c r="D165" s="9" t="s">
         <v>15</v>
@@ -7408,13 +7417,13 @@
     </row>
     <row r="166" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A166" s="9" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B166" s="10" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C166" s="11" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D166" s="9" t="s">
         <v>15</v>
@@ -7440,10 +7449,10 @@
     </row>
     <row r="167" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A167" s="9" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B167" s="10" t="s">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="C167" s="11" t="s">
         <v>433</v>
@@ -7472,10 +7481,10 @@
     </row>
     <row r="168" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A168" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B168" s="10" t="s">
-        <v>476</v>
+        <v>456</v>
       </c>
       <c r="C168" s="11" t="s">
         <v>433</v>
@@ -7504,10 +7513,10 @@
     </row>
     <row r="169" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A169" s="9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B169" s="10" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C169" s="11" t="s">
         <v>433</v>
@@ -7536,10 +7545,10 @@
     </row>
     <row r="170" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A170" s="9" t="s">
-        <v>479</v>
+        <v>436</v>
       </c>
       <c r="B170" s="10" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="C170" s="11" t="s">
         <v>433</v>
@@ -7568,10 +7577,10 @@
     </row>
     <row r="171" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A171" s="9" t="s">
-        <v>437</v>
+        <v>479</v>
       </c>
       <c r="B171" s="10" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="C171" s="11" t="s">
         <v>433</v>
@@ -7600,10 +7609,10 @@
     </row>
     <row r="172" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A172" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B172" s="10" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C172" s="11" t="s">
         <v>433</v>
@@ -7632,10 +7641,10 @@
     </row>
     <row r="173" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A173" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B173" s="10" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C173" s="11" t="s">
         <v>433</v>
@@ -7664,10 +7673,10 @@
     </row>
     <row r="174" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A174" s="9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B174" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C174" s="11" t="s">
         <v>433</v>
@@ -7696,10 +7705,10 @@
     </row>
     <row r="175" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A175" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B175" s="10" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C175" s="11" t="s">
         <v>433</v>
@@ -7728,10 +7737,10 @@
     </row>
     <row r="176" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A176" s="9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B176" s="10" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C176" s="11" t="s">
         <v>433</v>
@@ -7760,10 +7769,10 @@
     </row>
     <row r="177" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A177" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B177" s="10" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C177" s="11" t="s">
         <v>433</v>
@@ -7792,10 +7801,10 @@
     </row>
     <row r="178" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A178" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B178" s="10" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C178" s="11" t="s">
         <v>433</v>
@@ -7824,10 +7833,10 @@
     </row>
     <row r="179" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A179" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B179" s="10" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C179" s="11" t="s">
         <v>433</v>
@@ -7856,10 +7865,10 @@
     </row>
     <row r="180" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A180" s="9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B180" s="10" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C180" s="11" t="s">
         <v>433</v>
@@ -7888,10 +7897,10 @@
     </row>
     <row r="181" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A181" s="9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B181" s="10" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C181" s="11" t="s">
         <v>433</v>
@@ -7920,10 +7929,10 @@
     </row>
     <row r="182" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A182" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B182" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C182" s="11" t="s">
         <v>433</v>
@@ -7952,10 +7961,10 @@
     </row>
     <row r="183" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A183" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B183" s="10" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C183" s="11" t="s">
         <v>433</v>
@@ -7984,10 +7993,10 @@
     </row>
     <row r="184" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A184" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B184" s="10" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C184" s="11" t="s">
         <v>433</v>
@@ -8016,10 +8025,10 @@
     </row>
     <row r="185" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A185" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B185" s="10" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C185" s="11" t="s">
         <v>433</v>
@@ -8048,10 +8057,10 @@
     </row>
     <row r="186" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A186" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B186" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C186" s="11" t="s">
         <v>433</v>
@@ -8080,10 +8089,10 @@
     </row>
     <row r="187" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A187" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B187" s="10" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C187" s="11" t="s">
         <v>433</v>
@@ -8112,10 +8121,10 @@
     </row>
     <row r="188" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A188" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B188" s="10" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C188" s="11" t="s">
         <v>433</v>
@@ -8144,13 +8153,13 @@
     </row>
     <row r="189" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A189" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B189" s="10" t="s">
-        <v>477</v>
+        <v>457</v>
       </c>
       <c r="C189" s="11" t="s">
-        <v>478</v>
+        <v>433</v>
       </c>
       <c r="D189" s="9" t="s">
         <v>15</v>
@@ -8174,47 +8183,47 @@
         <v>131</v>
       </c>
     </row>
-    <row r="190" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A190" s="13" t="s">
+    <row r="190" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A190" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="B190" s="10" t="s">
+        <v>477</v>
+      </c>
+      <c r="C190" s="11" t="s">
+        <v>478</v>
+      </c>
+      <c r="D190" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E190" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F190" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G190" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="H190" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I190" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J190" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A191" s="13" t="s">
         <v>481</v>
       </c>
-      <c r="B190" s="14" t="s">
+      <c r="B191" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="C190" s="14" t="s">
+      <c r="C191" s="14" t="s">
         <v>483</v>
-      </c>
-      <c r="D190" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E190" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="F190" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G190" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="H190" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I190" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="J190" s="15" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="191" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A191" s="13" t="s">
-        <v>484</v>
-      </c>
-      <c r="B191" s="14" t="s">
-        <v>489</v>
-      </c>
-      <c r="C191" s="13" t="s">
-        <v>503</v>
       </c>
       <c r="D191" s="15" t="s">
         <v>15</v>
@@ -8240,13 +8249,13 @@
     </row>
     <row r="192" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A192" s="13" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B192" s="14" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C192" s="13" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D192" s="15" t="s">
         <v>15</v>
@@ -8272,13 +8281,13 @@
     </row>
     <row r="193" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A193" s="13" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B193" s="14" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C193" s="13" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D193" s="15" t="s">
         <v>15</v>
@@ -8304,13 +8313,13 @@
     </row>
     <row r="194" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A194" s="13" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B194" s="14" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C194" s="13" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D194" s="15" t="s">
         <v>15</v>
@@ -8336,13 +8345,13 @@
     </row>
     <row r="195" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A195" s="13" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B195" s="14" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C195" s="13" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D195" s="15" t="s">
         <v>15</v>
@@ -8366,47 +8375,47 @@
         <v>131</v>
       </c>
     </row>
-    <row r="196" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A196" s="16" t="s">
+    <row r="196" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A196" s="13" t="s">
+        <v>488</v>
+      </c>
+      <c r="B196" s="14" t="s">
+        <v>493</v>
+      </c>
+      <c r="C196" s="13" t="s">
+        <v>507</v>
+      </c>
+      <c r="D196" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E196" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F196" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G196" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="H196" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I196" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J196" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A197" s="16" t="s">
         <v>496</v>
       </c>
-      <c r="B196" s="17" t="s">
+      <c r="B197" s="17" t="s">
         <v>494</v>
       </c>
-      <c r="C196" s="17" t="s">
+      <c r="C197" s="17" t="s">
         <v>495</v>
-      </c>
-      <c r="D196" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E196" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F196" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G196" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="H196" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I196" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="J196" s="18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="197" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A197" s="16" t="s">
-        <v>497</v>
-      </c>
-      <c r="B197" s="17" t="s">
-        <v>500</v>
-      </c>
-      <c r="C197" s="17" t="s">
-        <v>508</v>
       </c>
       <c r="D197" s="18" t="s">
         <v>15</v>
@@ -8432,13 +8441,13 @@
     </row>
     <row r="198" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A198" s="16" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B198" s="17" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C198" s="17" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D198" s="18" t="s">
         <v>15</v>
@@ -8464,13 +8473,13 @@
     </row>
     <row r="199" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A199" s="16" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B199" s="17" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C199" s="17" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D199" s="18" t="s">
         <v>15</v>
@@ -8491,6 +8500,38 @@
         <v>2</v>
       </c>
       <c r="J199" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A200" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="B200" s="17" t="s">
+        <v>502</v>
+      </c>
+      <c r="C200" s="17" t="s">
+        <v>510</v>
+      </c>
+      <c r="D200" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E200" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F200" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G200" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H200" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I200" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="J200" s="18" t="s">
         <v>131</v>
       </c>
     </row>

</xml_diff>